<commit_message>
Doc: Updated Time Sheet
</commit_message>
<xml_diff>
--- a/Release Planning/Release_2 planning.xlsx
+++ b/Release Planning/Release_2 planning.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\ITI\QA\Online-Mobile-Store-WebSite\Release Planning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AB473E4-9307-4C16-AA65-F2776243C30C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5B03F39-D991-4683-B1A5-BCCEDD51C887}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -455,7 +455,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -514,8 +514,11 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -525,12 +528,6 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -753,7 +750,7 @@
   <dimension ref="A1:E39"/>
   <sheetViews>
     <sheetView topLeftCell="A29" zoomScale="66" workbookViewId="0">
-      <selection activeCell="C32" sqref="C32"/>
+      <selection activeCell="E39" sqref="E39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -783,7 +780,7 @@
       </c>
     </row>
     <row r="2" spans="1:5" ht="39.950000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="23" t="s">
+      <c r="A2" s="24" t="s">
         <v>5</v>
       </c>
       <c r="B2" s="11" t="s">
@@ -795,12 +792,12 @@
       <c r="D2" s="13">
         <v>3</v>
       </c>
-      <c r="E2" s="26">
+      <c r="E2" s="22">
         <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="39.950000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="24"/>
+      <c r="A3" s="25"/>
       <c r="B3" s="14" t="s">
         <v>8</v>
       </c>
@@ -810,12 +807,12 @@
       <c r="D3" s="16">
         <v>3</v>
       </c>
-      <c r="E3" s="27">
+      <c r="E3" s="23">
         <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="39.950000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="24"/>
+      <c r="A4" s="25"/>
       <c r="B4" s="14" t="s">
         <v>9</v>
       </c>
@@ -825,12 +822,12 @@
       <c r="D4" s="16">
         <v>4</v>
       </c>
-      <c r="E4" s="27">
+      <c r="E4" s="23">
         <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="39.950000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="24"/>
+      <c r="A5" s="25"/>
       <c r="B5" s="14" t="s">
         <v>11</v>
       </c>
@@ -840,12 +837,12 @@
       <c r="D5" s="16">
         <v>4</v>
       </c>
-      <c r="E5" s="27">
+      <c r="E5" s="23">
         <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="39.950000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="24"/>
+      <c r="A6" s="25"/>
       <c r="B6" s="14" t="s">
         <v>13</v>
       </c>
@@ -855,12 +852,12 @@
       <c r="D6" s="16">
         <v>1</v>
       </c>
-      <c r="E6" s="27">
+      <c r="E6" s="23">
         <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="39.950000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="24"/>
+      <c r="A7" s="25"/>
       <c r="B7" s="14" t="s">
         <v>14</v>
       </c>
@@ -870,12 +867,12 @@
       <c r="D7" s="16">
         <v>1.5</v>
       </c>
-      <c r="E7" s="27">
+      <c r="E7" s="23">
         <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="39.950000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="24"/>
+      <c r="A8" s="25"/>
       <c r="B8" s="14" t="s">
         <v>16</v>
       </c>
@@ -885,12 +882,12 @@
       <c r="D8" s="16">
         <v>1</v>
       </c>
-      <c r="E8" s="27">
+      <c r="E8" s="23">
         <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="39.950000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="25"/>
+      <c r="A9" s="26"/>
       <c r="B9" s="14" t="s">
         <v>18</v>
       </c>
@@ -900,7 +897,7 @@
       <c r="D9" s="16">
         <v>1.5</v>
       </c>
-      <c r="E9" s="27">
+      <c r="E9" s="23">
         <v>1</v>
       </c>
     </row>
@@ -912,7 +909,7 @@
       <c r="E10" s="20"/>
     </row>
     <row r="11" spans="1:5" ht="39.950000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="23" t="s">
+      <c r="A11" s="24" t="s">
         <v>19</v>
       </c>
       <c r="B11" s="14" t="s">
@@ -924,12 +921,12 @@
       <c r="D11" s="16">
         <v>3</v>
       </c>
-      <c r="E11" s="27">
+      <c r="E11" s="23">
         <v>2</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="39.950000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="24"/>
+      <c r="A12" s="25"/>
       <c r="B12" s="14" t="s">
         <v>50</v>
       </c>
@@ -939,12 +936,12 @@
       <c r="D12" s="16">
         <v>3</v>
       </c>
-      <c r="E12" s="27">
+      <c r="E12" s="23">
         <v>3</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="39.950000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="24"/>
+      <c r="A13" s="25"/>
       <c r="B13" s="14" t="s">
         <v>51</v>
       </c>
@@ -954,12 +951,12 @@
       <c r="D13" s="16">
         <v>3</v>
       </c>
-      <c r="E13" s="27">
+      <c r="E13" s="23">
         <v>3</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="39.950000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="24"/>
+      <c r="A14" s="25"/>
       <c r="B14" s="14" t="s">
         <v>52</v>
       </c>
@@ -969,12 +966,12 @@
       <c r="D14" s="16">
         <v>4</v>
       </c>
-      <c r="E14" s="27">
+      <c r="E14" s="23">
         <v>2</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="39.950000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="24"/>
+      <c r="A15" s="25"/>
       <c r="B15" s="14" t="s">
         <v>20</v>
       </c>
@@ -984,12 +981,12 @@
       <c r="D15" s="16">
         <v>4</v>
       </c>
-      <c r="E15" s="27">
+      <c r="E15" s="23">
         <v>3</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="39.950000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="24"/>
+      <c r="A16" s="25"/>
       <c r="B16" s="14" t="s">
         <v>21</v>
       </c>
@@ -999,12 +996,12 @@
       <c r="D16" s="16">
         <v>1</v>
       </c>
-      <c r="E16" s="27">
+      <c r="E16" s="23">
         <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="39.950000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="24"/>
+      <c r="A17" s="25"/>
       <c r="B17" s="14" t="s">
         <v>22</v>
       </c>
@@ -1014,12 +1011,12 @@
       <c r="D17" s="16">
         <v>1</v>
       </c>
-      <c r="E17" s="27">
+      <c r="E17" s="23">
         <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="39.950000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="25"/>
+      <c r="A18" s="26"/>
       <c r="B18" s="14" t="s">
         <v>23</v>
       </c>
@@ -1029,7 +1026,7 @@
       <c r="D18" s="16">
         <v>1</v>
       </c>
-      <c r="E18" s="27">
+      <c r="E18" s="23">
         <v>1</v>
       </c>
     </row>
@@ -1041,7 +1038,7 @@
       <c r="E19" s="20"/>
     </row>
     <row r="20" spans="1:5" ht="39.950000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="23" t="s">
+      <c r="A20" s="24" t="s">
         <v>25</v>
       </c>
       <c r="B20" s="14" t="s">
@@ -1053,12 +1050,12 @@
       <c r="D20" s="16">
         <v>4</v>
       </c>
-      <c r="E20" s="27">
+      <c r="E20" s="23">
         <v>4</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="39.950000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="24"/>
+      <c r="A21" s="25"/>
       <c r="B21" s="14" t="s">
         <v>27</v>
       </c>
@@ -1068,12 +1065,12 @@
       <c r="D21" s="16">
         <v>3</v>
       </c>
-      <c r="E21" s="27">
+      <c r="E21" s="23">
         <v>4</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="39.950000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="24"/>
+      <c r="A22" s="25"/>
       <c r="B22" s="14" t="s">
         <v>28</v>
       </c>
@@ -1083,12 +1080,12 @@
       <c r="D22" s="16">
         <v>5</v>
       </c>
-      <c r="E22" s="27">
+      <c r="E22" s="23">
         <v>7</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="39.950000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="24"/>
+      <c r="A23" s="25"/>
       <c r="B23" s="14" t="s">
         <v>29</v>
       </c>
@@ -1098,12 +1095,12 @@
       <c r="D23" s="16">
         <v>3</v>
       </c>
-      <c r="E23" s="27">
+      <c r="E23" s="23">
         <v>3</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="39.950000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="24"/>
+      <c r="A24" s="25"/>
       <c r="B24" s="14" t="s">
         <v>30</v>
       </c>
@@ -1113,12 +1110,12 @@
       <c r="D24" s="16">
         <v>4</v>
       </c>
-      <c r="E24" s="27">
+      <c r="E24" s="23">
         <v>5</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="39.950000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="24"/>
+      <c r="A25" s="25"/>
       <c r="B25" s="14" t="s">
         <v>31</v>
       </c>
@@ -1128,12 +1125,12 @@
       <c r="D25" s="16">
         <v>4</v>
       </c>
-      <c r="E25" s="27">
+      <c r="E25" s="23">
         <v>3</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="39.950000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="24"/>
+      <c r="A26" s="25"/>
       <c r="B26" s="14" t="s">
         <v>53</v>
       </c>
@@ -1143,12 +1140,12 @@
       <c r="D26" s="16">
         <v>4</v>
       </c>
-      <c r="E26" s="27">
+      <c r="E26" s="23">
         <v>5</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="39.950000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="24"/>
+      <c r="A27" s="25"/>
       <c r="B27" s="14" t="s">
         <v>54</v>
       </c>
@@ -1158,12 +1155,12 @@
       <c r="D27" s="16">
         <v>1</v>
       </c>
-      <c r="E27" s="27">
+      <c r="E27" s="23">
         <v>1</v>
       </c>
     </row>
     <row r="28" spans="1:5" ht="39.950000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="24"/>
+      <c r="A28" s="25"/>
       <c r="B28" s="14" t="s">
         <v>32</v>
       </c>
@@ -1173,12 +1170,12 @@
       <c r="D28" s="16">
         <v>1</v>
       </c>
-      <c r="E28" s="27">
+      <c r="E28" s="23">
         <v>1</v>
       </c>
     </row>
     <row r="29" spans="1:5" ht="39.950000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="24"/>
+      <c r="A29" s="25"/>
       <c r="B29" s="14" t="s">
         <v>33</v>
       </c>
@@ -1188,12 +1185,12 @@
       <c r="D29" s="16">
         <v>1</v>
       </c>
-      <c r="E29" s="27">
+      <c r="E29" s="23">
         <v>1</v>
       </c>
     </row>
     <row r="30" spans="1:5" ht="39.950000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="24"/>
+      <c r="A30" s="25"/>
       <c r="B30" s="14" t="s">
         <v>34</v>
       </c>
@@ -1203,12 +1200,12 @@
       <c r="D30" s="16">
         <v>1</v>
       </c>
-      <c r="E30" s="27">
+      <c r="E30" s="23">
         <v>1</v>
       </c>
     </row>
     <row r="31" spans="1:5" ht="39.950000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="24"/>
+      <c r="A31" s="25"/>
       <c r="B31" s="14" t="s">
         <v>35</v>
       </c>
@@ -1218,12 +1215,12 @@
       <c r="D31" s="16">
         <v>1</v>
       </c>
-      <c r="E31" s="27">
+      <c r="E31" s="23">
         <v>1</v>
       </c>
     </row>
     <row r="32" spans="1:5" ht="39.950000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A32" s="24"/>
+      <c r="A32" s="25"/>
       <c r="B32" s="14" t="s">
         <v>36</v>
       </c>
@@ -1233,12 +1230,12 @@
       <c r="D32" s="16">
         <v>1</v>
       </c>
-      <c r="E32" s="27">
+      <c r="E32" s="23">
         <v>1</v>
       </c>
     </row>
     <row r="33" spans="1:5" ht="39.950000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="25"/>
+      <c r="A33" s="26"/>
       <c r="B33" s="14" t="s">
         <v>37</v>
       </c>
@@ -1248,7 +1245,7 @@
       <c r="D33" s="16">
         <v>1</v>
       </c>
-      <c r="E33" s="27">
+      <c r="E33" s="23">
         <v>0.5</v>
       </c>
     </row>
@@ -1260,7 +1257,7 @@
       <c r="E34" s="19"/>
     </row>
     <row r="35" spans="1:5" ht="39.950000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A35" s="23" t="s">
+      <c r="A35" s="24" t="s">
         <v>55</v>
       </c>
       <c r="B35" s="14" t="s">
@@ -1277,7 +1274,7 @@
       </c>
     </row>
     <row r="36" spans="1:5" ht="39.950000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A36" s="24"/>
+      <c r="A36" s="25"/>
       <c r="B36" s="14" t="s">
         <v>39</v>
       </c>
@@ -1292,7 +1289,7 @@
       </c>
     </row>
     <row r="37" spans="1:5" ht="39.950000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A37" s="24"/>
+      <c r="A37" s="25"/>
       <c r="B37" s="14" t="s">
         <v>40</v>
       </c>
@@ -1307,7 +1304,7 @@
       </c>
     </row>
     <row r="38" spans="1:5" ht="39.950000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A38" s="25"/>
+      <c r="A38" s="26"/>
       <c r="B38" s="14" t="s">
         <v>41</v>
       </c>
@@ -1334,7 +1331,9 @@
       <c r="D39" s="16">
         <v>2</v>
       </c>
-      <c r="E39" s="22"/>
+      <c r="E39" s="17">
+        <v>4</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -1355,7 +1354,7 @@
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1391,7 +1390,7 @@
         <v>22</v>
       </c>
       <c r="D2" s="5">
-        <v>22</v>
+        <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1460,7 +1459,9 @@
       <c r="C7" s="10">
         <v>79</v>
       </c>
-      <c r="D7" s="10"/>
+      <c r="D7" s="10">
+        <v>84</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>